<commit_message>
lacks Springer,SD and PeerJ
</commit_message>
<xml_diff>
--- a/artigos_IJDC/SelecaoFase1 - Saulo.xlsx
+++ b/artigos_IJDC/SelecaoFase1 - Saulo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t xml:space="preserve">Revisiting the Data Lifecycle with Big Data Curation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aceito</t>
   </si>
   <si>
     <t xml:space="preserve">ACM</t>
@@ -176,17 +179,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -227,8 +226,8 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -269,30 +268,31 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="0" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>2015</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G2" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="J2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="0" t="s">
         <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>2009</v>
@@ -301,17 +301,15 @@
         <v>5</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="2"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="0" t="s">
         <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>2011</v>
@@ -320,17 +318,15 @@
         <v>5</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="2"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="0" t="s">
         <v>18</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>2007</v>
@@ -339,22 +335,22 @@
         <v>5</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="2"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="0" t="s">
         <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>2017</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="F6" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -388,7 +384,7 @@
   <sheetData>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>